<commit_message>
mearged tables in one database
</commit_message>
<xml_diff>
--- a/instance/convert.xlsx
+++ b/instance/convert.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VRUNDA PATEL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\harry_hermione_ron\website\instance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FECD8D-4304-43EE-AA1E-16CC3D44217E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCAF6DE-03D9-411C-904D-6DE7F86DFEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
   <si>
     <t>beasts</t>
   </si>
@@ -355,11 +355,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -676,33 +676,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D59E3E-6514-47D8-8557-E73EAB959FB6}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.54296875" customWidth="1"/>
     <col min="2" max="2" width="32.1796875" customWidth="1"/>
-    <col min="3" max="3" width="40.08984375" customWidth="1"/>
-    <col min="4" max="4" width="33.08984375" customWidth="1"/>
-    <col min="5" max="5" width="47.453125" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" customWidth="1"/>
+    <col min="3" max="4" width="40.08984375" customWidth="1"/>
+    <col min="5" max="5" width="33.08984375" customWidth="1"/>
+    <col min="6" max="6" width="47.453125" customWidth="1"/>
+    <col min="7" max="7" width="24.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -713,19 +714,22 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -735,20 +739,20 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -758,20 +762,20 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -781,20 +785,20 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -804,20 +808,20 @@
       <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -827,20 +831,20 @@
       <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -850,20 +854,20 @@
       <c r="C8" t="s">
         <v>39</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>41</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -873,20 +877,20 @@
       <c r="C9" t="s">
         <v>45</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>46</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>47</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -896,20 +900,20 @@
       <c r="C10" t="s">
         <v>51</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>52</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>53</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -919,20 +923,20 @@
       <c r="C11" t="s">
         <v>57</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>58</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>59</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -942,20 +946,20 @@
       <c r="C12" t="s">
         <v>63</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>64</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>65</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -965,20 +969,20 @@
       <c r="C13" t="s">
         <v>69</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>70</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>71</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -988,18 +992,18 @@
       <c r="C14" t="s">
         <v>75</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>76</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>77</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -1009,36 +1013,36 @@
       <c r="C15" t="s">
         <v>81</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>82</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>83</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G16" s="2"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" display="https://th.bing.com/th/id/R.fa385930af77ee7a1225f7093b09569b?rik=4W4tiXRbyQ7lIg&amp;riu=http%3a%2f%2fmedia-cache-ak0.pinimg.com%2f1200x%2f2c%2f9c%2ffd%2f2c9cfd90b6bdc31da72013bd004a3402.jpg&amp;ehk=ZdvCDcvV%2fzXJWIszU8VKIw%2bZeHylQfhR80tGsCThL2Q%3d&amp;risl=&amp;pid=ImgRaw&amp;r=0" xr:uid="{2F5FB499-FF30-4D27-AADF-6753D83AB872}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{E7723538-1062-4845-9999-C6DF80B2D56B}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{56E316F2-DC33-4615-B5F6-BF714E5F4E45}"/>
-    <hyperlink ref="G6" r:id="rId4" xr:uid="{D54F9BE9-1C3E-4EF0-9C39-0EF58BBC169A}"/>
-    <hyperlink ref="G7" r:id="rId5" xr:uid="{EB588345-E9D1-422D-BB0B-6743BC448F4D}"/>
-    <hyperlink ref="G8" r:id="rId6" xr:uid="{6E366BD5-7F13-4827-9349-ED270C02AA61}"/>
-    <hyperlink ref="G9" r:id="rId7" xr:uid="{5D835903-4A58-408B-A57D-E977754A6A27}"/>
-    <hyperlink ref="G10" r:id="rId8" xr:uid="{EDC903D6-238F-42E6-B8E2-B3393CDF270C}"/>
-    <hyperlink ref="G11" r:id="rId9" xr:uid="{ECEFE583-4BFD-42DD-9162-73624C266B5C}"/>
-    <hyperlink ref="G13" r:id="rId10" xr:uid="{B4BDA0D0-D4FD-4884-A5D7-CBC9D8DB5099}"/>
-    <hyperlink ref="G12" r:id="rId11" xr:uid="{B8C26564-6F2B-4D5A-B996-46133D44B542}"/>
+    <hyperlink ref="H3" r:id="rId1" display="https://th.bing.com/th/id/R.fa385930af77ee7a1225f7093b09569b?rik=4W4tiXRbyQ7lIg&amp;riu=http%3a%2f%2fmedia-cache-ak0.pinimg.com%2f1200x%2f2c%2f9c%2ffd%2f2c9cfd90b6bdc31da72013bd004a3402.jpg&amp;ehk=ZdvCDcvV%2fzXJWIszU8VKIw%2bZeHylQfhR80tGsCThL2Q%3d&amp;risl=&amp;pid=ImgRaw&amp;r=0" xr:uid="{2F5FB499-FF30-4D27-AADF-6753D83AB872}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{E7723538-1062-4845-9999-C6DF80B2D56B}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{56E316F2-DC33-4615-B5F6-BF714E5F4E45}"/>
+    <hyperlink ref="H6" r:id="rId4" xr:uid="{D54F9BE9-1C3E-4EF0-9C39-0EF58BBC169A}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{EB588345-E9D1-422D-BB0B-6743BC448F4D}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{6E366BD5-7F13-4827-9349-ED270C02AA61}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{5D835903-4A58-408B-A57D-E977754A6A27}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{EDC903D6-238F-42E6-B8E2-B3393CDF270C}"/>
+    <hyperlink ref="H11" r:id="rId9" xr:uid="{ECEFE583-4BFD-42DD-9162-73624C266B5C}"/>
+    <hyperlink ref="H13" r:id="rId10" xr:uid="{B4BDA0D0-D4FD-4884-A5D7-CBC9D8DB5099}"/>
+    <hyperlink ref="H12" r:id="rId11" xr:uid="{B8C26564-6F2B-4D5A-B996-46133D44B542}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId12"/>

</xml_diff>